<commit_message>
use ARIMA to fit the Gordon Model
</commit_message>
<xml_diff>
--- a/séries_AirLiquide.xlsx
+++ b/séries_AirLiquide.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal_projects\Finance\dividend-model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal_projects\Finance\DividendModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBECBC71-5252-4523-9CAF-38B14F42EC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A29CE70-CBA6-4BBB-B548-9780BB9EFA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="part1" sheetId="1" r:id="rId1"/>
+    <sheet name="part2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="405">
   <si>
     <t>1987M03</t>
   </si>
@@ -1225,13 +1225,25 @@
   </si>
   <si>
     <t>Indice CAC40</t>
+  </si>
+  <si>
+    <t>CAC40_basis_points</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>Dividend</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1239,13 +1251,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1260,8 +1291,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1570,7 +1608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D398"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -7157,12 +7195,74 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2.492</v>
+      </c>
+      <c r="C2" s="2">
+        <v>127.883</v>
+      </c>
+      <c r="D2" s="2">
+        <v>5735.8429999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2021</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="C3" s="3">
+        <v>139.38</v>
+      </c>
+      <c r="D3" s="3">
+        <v>5256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2022</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2.6360000000000001</v>
+      </c>
+      <c r="C4" s="3">
+        <v>134.69999999999999</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3942</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>